<commit_message>
xD fotos y mas
</commit_message>
<xml_diff>
--- a/BDD/registros/Administradores.xlsx
+++ b/BDD/registros/Administradores.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="23040" windowHeight="9732"/>
+    <workbookView windowWidth="23040" windowHeight="9287"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -1175,7 +1175,7 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelRow="3" outlineLevelCol="1"/>
@@ -1192,17 +1192,26 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="2:2">
+    <row r="2" spans="1:2">
+      <c r="A2">
+        <v>1</v>
+      </c>
       <c r="B2">
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="2:2">
+    <row r="3" spans="1:2">
+      <c r="A3">
+        <v>2</v>
+      </c>
       <c r="B3">
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="2:2">
+    <row r="4" spans="1:2">
+      <c r="A4">
+        <v>3</v>
+      </c>
       <c r="B4">
         <v>15</v>
       </c>

</xml_diff>